<commit_message>
Modification excel et raml
</commit_message>
<xml_diff>
--- a/user-resource-description.xlsx
+++ b/user-resource-description.xlsx
@@ -165,13 +165,13 @@
     <t>User (id, firstname, lastname, phon, role)</t>
   </si>
   <si>
-    <t>Issue (id, author, type, description, coordonées, comment, status, action)</t>
-  </si>
-  <si>
     <t>IssueType (id, shortName, description)</t>
   </si>
   <si>
     <t>Action (id, actionName, description, author)</t>
+  </si>
+  <si>
+    <t>Issue (id, author, type, description, coords, comment, status, action)</t>
   </si>
 </sst>
 </file>
@@ -540,24 +540,39 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -569,9 +584,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -579,53 +591,41 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="57">
@@ -1020,7 +1020,7 @@
   <dimension ref="A2:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:A31"/>
+      <selection activeCell="A11" sqref="A11:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1034,43 +1034,43 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="33" customHeight="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="15" t="s">
+      <c r="E2" s="19"/>
+      <c r="F2" s="20" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="33" customHeight="1">
-      <c r="A3" s="13"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
       <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="16"/>
+      <c r="F3" s="21"/>
     </row>
     <row r="4" spans="1:6" ht="33" customHeight="1">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="16" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -1079,37 +1079,37 @@
       <c r="E4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="18" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="33" customHeight="1">
-      <c r="A5" s="20"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
+      <c r="A5" s="24"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
       <c r="D5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="9"/>
+      <c r="F5" s="18"/>
     </row>
     <row r="6" spans="1:6" ht="33" customHeight="1">
-      <c r="A6" s="20"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
       <c r="D6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="9"/>
+      <c r="F6" s="18"/>
     </row>
     <row r="7" spans="1:6" ht="33" customHeight="1">
-      <c r="A7" s="20"/>
-      <c r="B7" s="8"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="16"/>
       <c r="C7" s="4" t="s">
         <v>12</v>
       </c>
@@ -1124,8 +1124,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="33" customHeight="1">
-      <c r="A8" s="20"/>
-      <c r="B8" s="8" t="s">
+      <c r="A8" s="24"/>
+      <c r="B8" s="16" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -1142,8 +1142,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="33" customHeight="1">
-      <c r="A9" s="20"/>
-      <c r="B9" s="8"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="16"/>
       <c r="C9" s="4" t="s">
         <v>19</v>
       </c>
@@ -1158,69 +1158,69 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="33" customHeight="1" thickBot="1">
-      <c r="A10" s="22"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="24" t="s">
+      <c r="A10" s="25"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="26" t="s">
+      <c r="D10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="11" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="25" customHeight="1">
-      <c r="A11" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="28" t="s">
+      <c r="A11" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="31" t="s">
+      <c r="E11" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="32" t="s">
+      <c r="F11" s="33" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" customHeight="1">
-      <c r="A12" s="20"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="10"/>
+      <c r="A12" s="24"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="36"/>
       <c r="D12" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="9"/>
+      <c r="F12" s="18"/>
     </row>
     <row r="13" spans="1:6" ht="26" customHeight="1">
-      <c r="A13" s="20"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="10"/>
+      <c r="A13" s="24"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="36"/>
       <c r="D13" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="9"/>
+      <c r="F13" s="18"/>
     </row>
     <row r="14" spans="1:6" ht="26" customHeight="1">
-      <c r="A14" s="20"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="10"/>
+      <c r="A14" s="24"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="36"/>
       <c r="D14" s="4" t="s">
         <v>29</v>
       </c>
@@ -1232,9 +1232,9 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="26" customHeight="1">
-      <c r="A15" s="20"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="11"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="26"/>
       <c r="D15" s="4" t="s">
         <v>5</v>
       </c>
@@ -1244,8 +1244,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="18">
-      <c r="A16" s="20"/>
-      <c r="B16" s="8"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="16"/>
       <c r="C16" s="4" t="s">
         <v>12</v>
       </c>
@@ -1260,8 +1260,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="18">
-      <c r="A17" s="20"/>
-      <c r="B17" s="8" t="s">
+      <c r="A17" s="24"/>
+      <c r="B17" s="16" t="s">
         <v>36</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -1278,8 +1278,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1">
-      <c r="A18" s="20"/>
-      <c r="B18" s="8"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="16"/>
       <c r="C18" s="4" t="s">
         <v>19</v>
       </c>
@@ -1294,68 +1294,68 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" thickBot="1">
-      <c r="A19" s="22"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="24" t="s">
+      <c r="A19" s="25"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="F19" s="26" t="s">
+      <c r="D19" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="18">
-      <c r="A20" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" s="28" t="s">
+      <c r="A20" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="28" t="s">
+      <c r="C20" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="30" t="s">
+      <c r="D20" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="31" t="s">
+      <c r="E20" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="32" t="s">
+      <c r="F20" s="33" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="18">
-      <c r="A21" s="34"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
       <c r="D21" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F21" s="9"/>
+      <c r="F21" s="18"/>
     </row>
     <row r="22" spans="1:6" ht="18">
-      <c r="A22" s="34"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
       <c r="D22" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="9"/>
+      <c r="F22" s="18"/>
     </row>
     <row r="23" spans="1:6" ht="18">
-      <c r="A23" s="34"/>
-      <c r="B23" s="8"/>
+      <c r="A23" s="29"/>
+      <c r="B23" s="16"/>
       <c r="C23" s="4" t="s">
         <v>12</v>
       </c>
@@ -1370,8 +1370,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="18">
-      <c r="A24" s="34"/>
-      <c r="B24" s="8" t="s">
+      <c r="A24" s="29"/>
+      <c r="B24" s="16" t="s">
         <v>38</v>
       </c>
       <c r="C24" s="4" t="s">
@@ -1388,8 +1388,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="18">
-      <c r="A25" s="34"/>
-      <c r="B25" s="8"/>
+      <c r="A25" s="29"/>
+      <c r="B25" s="16"/>
       <c r="C25" s="4" t="s">
         <v>19</v>
       </c>
@@ -1404,68 +1404,68 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="19" thickBot="1">
-      <c r="A26" s="35"/>
-      <c r="B26" s="23"/>
-      <c r="C26" s="24" t="s">
+      <c r="A26" s="31"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D26" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="F26" s="26" t="s">
+      <c r="D26" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="11" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="18">
-      <c r="A27" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" s="11" t="s">
+      <c r="A27" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="26" t="s">
         <v>7</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E27" s="18" t="s">
+      <c r="E27" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F27" s="21" t="s">
+      <c r="F27" s="27" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="18">
-      <c r="A28" s="34"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
+      <c r="A28" s="29"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
       <c r="D28" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F28" s="9"/>
+      <c r="F28" s="18"/>
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1">
-      <c r="A29" s="34"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
+      <c r="A29" s="29"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
       <c r="D29" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F29" s="9"/>
+      <c r="F29" s="18"/>
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1">
-      <c r="A30" s="34"/>
-      <c r="B30" s="8"/>
+      <c r="A30" s="29"/>
+      <c r="B30" s="16"/>
       <c r="C30" s="4" t="s">
         <v>12</v>
       </c>
@@ -1480,7 +1480,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="18">
-      <c r="A31" s="36"/>
+      <c r="A31" s="30"/>
       <c r="B31" s="4" t="s">
         <v>40</v>
       </c>
@@ -1502,6 +1502,20 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B11:B16"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="A11:A19"/>
+    <mergeCell ref="C11:C15"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="F27:F29"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="B24:B26"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B4:B7"/>
     <mergeCell ref="B8:B10"/>
@@ -1512,24 +1526,9 @@
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="A4:A10"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="F27:F29"/>
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="B11:B16"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="A11:A19"/>
-    <mergeCell ref="C11:C15"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>

<commit_message>
modification action et issue
</commit_message>
<xml_diff>
--- a/user-resource-description.xlsx
+++ b/user-resource-description.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -172,6 +172,12 @@
   </si>
   <si>
     <t>Issue (id, author, type, description, coords, action)</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Retrieve a list of issue by Action</t>
   </si>
 </sst>
 </file>
@@ -458,7 +464,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="57">
+  <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -516,8 +522,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -558,77 +566,83 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="57">
+  <cellStyles count="59">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="5" builtinId="8" hidden="1"/>
@@ -657,6 +671,7 @@
     <cellStyle name="Collegamento ipertestuale" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="6" builtinId="9" hidden="1"/>
@@ -685,6 +700,7 @@
     <cellStyle name="Collegamento visitato" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1017,10 +1033,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:F32"/>
+  <dimension ref="A2:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:A19"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1034,43 +1050,43 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="33" customHeight="1">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="32"/>
-      <c r="F2" s="33" t="s">
+      <c r="E2" s="21"/>
+      <c r="F2" s="22" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="33" customHeight="1">
-      <c r="A3" s="31"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
       <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="34"/>
+      <c r="F3" s="23"/>
     </row>
     <row r="4" spans="1:6" ht="33" customHeight="1">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="18" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -1079,37 +1095,37 @@
       <c r="E4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="20" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="33" customHeight="1">
-      <c r="A5" s="20"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
       <c r="D5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="20"/>
     </row>
     <row r="6" spans="1:6" ht="33" customHeight="1">
-      <c r="A6" s="20"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
       <c r="D6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="17"/>
+      <c r="F6" s="20"/>
     </row>
     <row r="7" spans="1:6" ht="33" customHeight="1">
-      <c r="A7" s="20"/>
-      <c r="B7" s="15"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="18"/>
       <c r="C7" s="4" t="s">
         <v>12</v>
       </c>
@@ -1124,8 +1140,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="33" customHeight="1">
-      <c r="A8" s="20"/>
-      <c r="B8" s="15" t="s">
+      <c r="A8" s="26"/>
+      <c r="B8" s="18" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -1142,8 +1158,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="33" customHeight="1">
-      <c r="A9" s="20"/>
-      <c r="B9" s="15"/>
+      <c r="A9" s="26"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="4" t="s">
         <v>19</v>
       </c>
@@ -1158,8 +1174,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="33" customHeight="1" thickBot="1">
-      <c r="A10" s="21"/>
-      <c r="B10" s="18"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="19"/>
       <c r="C10" s="9" t="s">
         <v>20</v>
       </c>
@@ -1174,13 +1190,13 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="25" customHeight="1">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="37" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="12" t="s">
@@ -1189,38 +1205,38 @@
       <c r="E11" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="35" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" customHeight="1">
-      <c r="A12" s="20"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="23"/>
+      <c r="A12" s="26"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="38"/>
       <c r="D12" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="17"/>
+      <c r="F12" s="20"/>
     </row>
     <row r="13" spans="1:6" ht="26" customHeight="1">
-      <c r="A13" s="20"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="23"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="38"/>
       <c r="D13" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="17"/>
+      <c r="F13" s="20"/>
     </row>
     <row r="14" spans="1:6" ht="26" customHeight="1">
-      <c r="A14" s="20"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="23"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="38"/>
       <c r="D14" s="4" t="s">
         <v>29</v>
       </c>
@@ -1232,276 +1248,302 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="26" customHeight="1">
-      <c r="A15" s="20"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="4" t="s">
+      <c r="A15" s="26"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="26" customHeight="1">
+      <c r="A16" s="26"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="5" t="s">
+      <c r="E16" s="2"/>
+      <c r="F16" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="18">
-      <c r="A16" s="20"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="4" t="s">
+    <row r="17" spans="1:6" ht="18">
+      <c r="A17" s="26"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="5" t="s">
+      <c r="D17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="18">
-      <c r="A17" s="20"/>
-      <c r="B17" s="15" t="s">
+    <row r="18" spans="1:6" ht="18">
+      <c r="A18" s="26"/>
+      <c r="B18" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="2" t="s">
+      <c r="D18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1">
-      <c r="A18" s="20"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="4" t="s">
+    <row r="19" spans="1:6" ht="15" customHeight="1">
+      <c r="A19" s="26"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" s="2" t="s">
+      <c r="D19" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" thickBot="1">
-      <c r="A19" s="21"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="9" t="s">
+    <row r="20" spans="1:6" ht="15" customHeight="1" thickBot="1">
+      <c r="A20" s="27"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F19" s="11" t="s">
+      <c r="D20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="18">
-      <c r="A20" s="26" t="s">
+    <row r="21" spans="1:6" ht="18">
+      <c r="A21" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B21" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C21" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D21" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="E21" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="16" t="s">
+      <c r="F21" s="35" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="18">
-      <c r="A21" s="27"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="4" t="s">
+    <row r="22" spans="1:6" ht="18">
+      <c r="A22" s="31"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F21" s="17"/>
-    </row>
-    <row r="22" spans="1:6" ht="18">
-      <c r="A22" s="27"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="4" t="s">
+      <c r="F22" s="20"/>
+    </row>
+    <row r="23" spans="1:6" ht="18">
+      <c r="A23" s="31"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="17"/>
-    </row>
-    <row r="23" spans="1:6" ht="18">
-      <c r="A23" s="27"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="4" t="s">
+      <c r="F23" s="20"/>
+    </row>
+    <row r="24" spans="1:6" ht="18">
+      <c r="A24" s="31"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" s="5" t="s">
+      <c r="D24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="18">
-      <c r="A24" s="27"/>
-      <c r="B24" s="15" t="s">
+    <row r="25" spans="1:6" ht="18">
+      <c r="A25" s="31"/>
+      <c r="B25" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C25" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F24" s="2" t="s">
+      <c r="D25" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="18">
-      <c r="A25" s="27"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="4" t="s">
+    <row r="26" spans="1:6" ht="18">
+      <c r="A26" s="31"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F25" s="2" t="s">
+      <c r="D26" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="19" thickBot="1">
-      <c r="A26" s="29"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="9" t="s">
+    <row r="27" spans="1:6" ht="19" thickBot="1">
+      <c r="A27" s="33"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D26" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F26" s="11" t="s">
+      <c r="D27" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="18">
-      <c r="A27" s="26" t="s">
+    <row r="28" spans="1:6" ht="18">
+      <c r="A28" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="24" t="s">
+      <c r="B28" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="24" t="s">
+      <c r="C28" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D28" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E28" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F27" s="25" t="s">
+      <c r="F28" s="29" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="18">
-      <c r="A28" s="27"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="4" t="s">
+    <row r="29" spans="1:6" ht="18">
+      <c r="A29" s="31"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F28" s="17"/>
-    </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1">
-      <c r="A29" s="27"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="4" t="s">
+      <c r="F29" s="20"/>
+    </row>
+    <row r="30" spans="1:6" ht="15" customHeight="1">
+      <c r="A30" s="31"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F29" s="17"/>
-    </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1">
-      <c r="A30" s="27"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="4" t="s">
+      <c r="F30" s="20"/>
+    </row>
+    <row r="31" spans="1:6" ht="15" customHeight="1">
+      <c r="A31" s="31"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F30" s="5" t="s">
+      <c r="D31" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="18">
-      <c r="A31" s="28"/>
-      <c r="B31" s="4" t="s">
+    <row r="32" spans="1:6" ht="18">
+      <c r="A32" s="32"/>
+      <c r="B32" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C32" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F31" s="2" t="s">
+      <c r="D32" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1">
-      <c r="A32" s="7"/>
+    <row r="33" spans="1:1" ht="15" customHeight="1">
+      <c r="A33" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B11:B17"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="A11:A20"/>
+    <mergeCell ref="C11:C16"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="F28:F30"/>
+    <mergeCell ref="A28:A32"/>
+    <mergeCell ref="A21:A27"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="B25:B27"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B4:B7"/>
     <mergeCell ref="B8:B10"/>
@@ -1512,23 +1554,10 @@
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="A4:A10"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="F27:F29"/>
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="B11:B16"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="A11:A19"/>
-    <mergeCell ref="C11:C15"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>